<commit_message>
add examples and FB Likes
</commit_message>
<xml_diff>
--- a/data/example/C03/C03E04 - Year per Worksheet.xlsx
+++ b/data/example/C03/C03E04 - Year per Worksheet.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gil.raviv\OneDrive - Data Chant\Book\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\C03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="425D15BBAD0365E79896D2932690B4134E2300D2" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D944834B-74D4-47FD-9B68-95A7BB0019F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11110" windowHeight="5930" xr2:uid="{05DCDE0C-BE15-4CB6-BF49-566382761ADC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{05DCDE0C-BE15-4CB6-BF49-566382761ADC}"/>
   </bookViews>
   <sheets>
-    <sheet name="2015" sheetId="1" r:id="rId1"/>
-    <sheet name="2016" sheetId="2" r:id="rId2"/>
-    <sheet name="2017" sheetId="3" r:id="rId3"/>
+    <sheet name="2014" sheetId="4" r:id="rId1"/>
+    <sheet name="2015" sheetId="1" r:id="rId2"/>
+    <sheet name="2016" sheetId="2" r:id="rId3"/>
+    <sheet name="2017" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="663">
   <si>
     <t>Name</t>
   </si>
@@ -2022,11 +2023,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2034,8 +2035,15 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2162,7 +2170,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2178,7 +2186,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2473,16 +2481,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5245E30E-D694-47C0-A25D-591F0C4E79FE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19CDAC0A-5196-4393-92DD-90EE2E1BA55E}">
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2511,7 +2519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>514</v>
       </c>
@@ -2540,7 +2548,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>516</v>
       </c>
@@ -2569,7 +2577,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>518</v>
       </c>
@@ -2598,7 +2606,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>291</v>
       </c>
@@ -2623,7 +2631,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>648</v>
       </c>
@@ -2648,7 +2656,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>651</v>
       </c>
@@ -2675,7 +2683,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>653</v>
       </c>
@@ -2702,7 +2710,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>655</v>
       </c>
@@ -2729,7 +2737,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>657</v>
       </c>
@@ -2756,7 +2764,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>520</v>
       </c>
@@ -2785,7 +2793,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>522</v>
       </c>
@@ -2814,7 +2822,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>524</v>
       </c>
@@ -2843,7 +2851,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>526</v>
       </c>
@@ -2872,7 +2880,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>528</v>
       </c>
@@ -2901,7 +2909,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>530</v>
       </c>
@@ -2930,7 +2938,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>532</v>
       </c>
@@ -2959,7 +2967,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>534</v>
       </c>
@@ -2988,7 +2996,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>294</v>
       </c>
@@ -3013,7 +3021,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>296</v>
       </c>
@@ -3038,7 +3046,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>536</v>
       </c>
@@ -3067,7 +3075,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>538</v>
       </c>
@@ -3096,7 +3104,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>540</v>
       </c>
@@ -3125,7 +3133,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>542</v>
       </c>
@@ -3154,7 +3162,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>544</v>
       </c>
@@ -3183,7 +3191,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>546</v>
       </c>
@@ -3212,7 +3220,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>548</v>
       </c>
@@ -3241,7 +3249,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>550</v>
       </c>
@@ -3270,7 +3278,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>552</v>
       </c>
@@ -3299,7 +3307,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>554</v>
       </c>
@@ -3328,7 +3336,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>659</v>
       </c>
@@ -3355,7 +3363,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>661</v>
       </c>
@@ -3382,7 +3390,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>556</v>
       </c>
@@ -3411,7 +3419,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>558</v>
       </c>
@@ -3440,7 +3448,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>560</v>
       </c>
@@ -3469,7 +3477,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>562</v>
       </c>
@@ -3498,7 +3506,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>564</v>
       </c>
@@ -3527,7 +3535,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>164</v>
       </c>
@@ -3556,7 +3564,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>166</v>
       </c>
@@ -3585,7 +3593,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>168</v>
       </c>
@@ -3614,7 +3622,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>170</v>
       </c>
@@ -3643,7 +3651,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>172</v>
       </c>
@@ -3672,7 +3680,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>175</v>
       </c>
@@ -3701,7 +3709,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>177</v>
       </c>
@@ -3730,7 +3738,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>179</v>
       </c>
@@ -3759,7 +3767,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>181</v>
       </c>
@@ -3788,7 +3796,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>183</v>
       </c>
@@ -3817,7 +3825,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>185</v>
       </c>
@@ -3846,7 +3854,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
         <v>187</v>
       </c>
@@ -3875,7 +3883,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>189</v>
       </c>
@@ -3904,7 +3912,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
         <v>191</v>
       </c>
@@ -3933,7 +3941,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>193</v>
       </c>
@@ -3962,7 +3970,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
         <v>195</v>
       </c>
@@ -3991,7 +3999,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>197</v>
       </c>
@@ -4020,7 +4028,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>199</v>
       </c>
@@ -4049,7 +4057,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>201</v>
       </c>
@@ -4078,7 +4086,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>203</v>
       </c>
@@ -4107,7 +4115,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>205</v>
       </c>
@@ -4136,7 +4144,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>207</v>
       </c>
@@ -4165,7 +4173,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>209</v>
       </c>
@@ -4194,7 +4202,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
         <v>211</v>
       </c>
@@ -4223,7 +4231,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>213</v>
       </c>
@@ -4252,7 +4260,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
         <v>215</v>
       </c>
@@ -4281,7 +4289,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>217</v>
       </c>
@@ -4310,7 +4318,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
         <v>219</v>
       </c>
@@ -4339,7 +4347,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>221</v>
       </c>
@@ -4368,7 +4376,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
         <v>223</v>
       </c>
@@ -4397,7 +4405,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>566</v>
       </c>
@@ -4426,7 +4434,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>568</v>
       </c>
@@ -4455,7 +4463,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>570</v>
       </c>
@@ -4484,7 +4492,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
         <v>572</v>
       </c>
@@ -4513,7 +4521,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>574</v>
       </c>
@@ -4542,7 +4550,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
         <v>576</v>
       </c>
@@ -4572,19 +4580,2125 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5245E30E-D694-47C0-A25D-591F0C4E79FE}">
+  <dimension ref="A1:I73"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="6">
+        <v>739.04100000000005</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1349.6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1288.2</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="10">
+        <v>739.04100000000005</v>
+      </c>
+      <c r="E3" s="10">
+        <v>1349.6</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="10">
+        <v>1215.6199999999999</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="6">
+        <v>747.2002</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1364.5</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1215.6199999999999</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="10">
+        <v>13.0863</v>
+      </c>
+      <c r="E5" s="10">
+        <v>34.99</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="D6" s="6">
+        <v>6.9222999999999999</v>
+      </c>
+      <c r="E6" s="6">
+        <v>8.99</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>651</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>642</v>
+      </c>
+      <c r="D7" s="10">
+        <v>38.4923</v>
+      </c>
+      <c r="E7" s="10">
+        <v>49.99</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>580</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="D8" s="6">
+        <v>38.4923</v>
+      </c>
+      <c r="E8" s="6">
+        <v>49.99</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>642</v>
+      </c>
+      <c r="D9" s="10">
+        <v>38.4923</v>
+      </c>
+      <c r="E9" s="10">
+        <v>49.99</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>658</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="D10" s="6">
+        <v>38.4923</v>
+      </c>
+      <c r="E10" s="6">
+        <v>49.99</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>521</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="10">
+        <v>868.63419999999996</v>
+      </c>
+      <c r="E11" s="10">
+        <v>1431.5</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="10">
+        <v>1043.26</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="6">
+        <v>868.63419999999996</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1431.5</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="6">
+        <v>961.61</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="10">
+        <v>868.63419999999996</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1431.5</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="10">
+        <v>979.75</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="6">
+        <v>868.63419999999996</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1431.5</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="6">
+        <v>997.9</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="10">
+        <v>868.63419999999996</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1431.5</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="G15" s="10">
+        <v>1016.04</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="6">
+        <v>204.6251</v>
+      </c>
+      <c r="E16" s="6">
+        <v>337.22</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1115.83</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="10">
+        <v>204.6251</v>
+      </c>
+      <c r="E17" s="10">
+        <v>337.22</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="10">
+        <v>1124.9000000000001</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="6">
+        <v>204.6251</v>
+      </c>
+      <c r="E18" s="6">
+        <v>337.22</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1133.98</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="10">
+        <v>13.0863</v>
+      </c>
+      <c r="E19" s="10">
+        <v>34.99</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="6">
+        <v>13.0863</v>
+      </c>
+      <c r="E20" s="6">
+        <v>34.99</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>536</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>537</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="10">
+        <v>204.6251</v>
+      </c>
+      <c r="E21" s="10">
+        <v>337.22</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="10">
+        <v>1052.33</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="6">
+        <v>204.6251</v>
+      </c>
+      <c r="E22" s="6">
+        <v>337.22</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="6">
+        <v>1070.47</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>540</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="10">
+        <v>204.6251</v>
+      </c>
+      <c r="E23" s="10">
+        <v>337.22</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="10">
+        <v>1088.6199999999999</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="6">
+        <v>747.2002</v>
+      </c>
+      <c r="E24" s="6">
+        <v>1364.5</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="6">
+        <v>1233.76</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>544</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>545</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="10">
+        <v>747.2002</v>
+      </c>
+      <c r="E25" s="10">
+        <v>1364.5</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="10">
+        <v>1288.2</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="6">
+        <v>739.04100000000005</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1349.6</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="6">
+        <v>1233.76</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>548</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="10">
+        <v>699.09280000000001</v>
+      </c>
+      <c r="E27" s="10">
+        <v>1349.6</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="10">
+        <v>1251.9100000000001</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="6">
+        <v>699.09280000000001</v>
+      </c>
+      <c r="E28" s="6">
+        <v>1349.6</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="6">
+        <v>1270.05</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>552</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="10">
+        <v>706.81100000000004</v>
+      </c>
+      <c r="E29" s="10">
+        <v>1364.5</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" s="10">
+        <v>1251.9100000000001</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="6">
+        <v>706.81100000000004</v>
+      </c>
+      <c r="E30" s="6">
+        <v>1364.5</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" s="6">
+        <v>1270.05</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>659</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="D31" s="10">
+        <v>3.3963000000000001</v>
+      </c>
+      <c r="E31" s="10">
+        <v>9.5</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="G31" s="10"/>
+      <c r="H31" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="D32" s="6">
+        <v>3.3963000000000001</v>
+      </c>
+      <c r="E32" s="6">
+        <v>9.5</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>556</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>557</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="10">
+        <v>352.13940000000002</v>
+      </c>
+      <c r="E33" s="10">
+        <v>594.83000000000004</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" s="10">
+        <v>1006.97</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D34" s="6">
+        <v>352.13940000000002</v>
+      </c>
+      <c r="E34" s="6">
+        <v>594.83000000000004</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G34" s="6">
+        <v>1025.1099999999999</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>560</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" s="10">
+        <v>352.13940000000002</v>
+      </c>
+      <c r="E35" s="10">
+        <v>594.83000000000004</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G35" s="10">
+        <v>1043.26</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="6">
+        <v>352.13940000000002</v>
+      </c>
+      <c r="E36" s="6">
+        <v>594.83000000000004</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G36" s="6">
+        <v>1070.47</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>564</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D37" s="10">
+        <v>352.13940000000002</v>
+      </c>
+      <c r="E37" s="10">
+        <v>594.83000000000004</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="10">
+        <v>1079.54</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" s="6">
+        <v>2171.2941999999998</v>
+      </c>
+      <c r="E38" s="6">
+        <v>3578.27</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" s="6">
+        <v>6803.85</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39" s="10">
+        <v>2171.2941999999998</v>
+      </c>
+      <c r="E39" s="10">
+        <v>3578.27</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G39" s="10">
+        <v>6245.93</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="6">
+        <v>2171.2941999999998</v>
+      </c>
+      <c r="E40" s="6">
+        <v>3578.27</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G40" s="6">
+        <v>6409.23</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" s="10">
+        <v>2171.2941999999998</v>
+      </c>
+      <c r="E41" s="10">
+        <v>3578.27</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G41" s="10">
+        <v>6540.77</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="6">
+        <v>2171.2941999999998</v>
+      </c>
+      <c r="E42" s="6">
+        <v>3578.27</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G42" s="6">
+        <v>6658.7</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" s="10">
+        <v>884.70830000000001</v>
+      </c>
+      <c r="E43" s="10">
+        <v>1457.99</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G43" s="10">
+        <v>8069.37</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="6">
+        <v>884.70830000000001</v>
+      </c>
+      <c r="E44" s="6">
+        <v>1457.99</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="6">
+        <v>8119.26</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" s="10">
+        <v>884.70830000000001</v>
+      </c>
+      <c r="E45" s="10">
+        <v>1457.99</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G45" s="10">
+        <v>7606.7</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" s="6">
+        <v>884.70830000000001</v>
+      </c>
+      <c r="E46" s="6">
+        <v>1457.99</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G46" s="6">
+        <v>7770</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="10">
+        <v>884.70830000000001</v>
+      </c>
+      <c r="E47" s="10">
+        <v>1457.99</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G47" s="10">
+        <v>7901.54</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="6">
+        <v>1912.1543999999999</v>
+      </c>
+      <c r="E48" s="6">
+        <v>3399.99</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G48" s="6">
+        <v>9230.56</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="10">
+        <v>1912.1543999999999</v>
+      </c>
+      <c r="E49" s="10">
+        <v>3399.99</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G49" s="10">
+        <v>9421.06</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" s="6">
+        <v>1912.1543999999999</v>
+      </c>
+      <c r="E50" s="6">
+        <v>3399.99</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G50" s="6">
+        <v>9584.36</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" s="10">
+        <v>1912.1543999999999</v>
+      </c>
+      <c r="E51" s="10">
+        <v>3399.99</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G51" s="10">
+        <v>9715.9</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I51" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" s="6">
+        <v>1898.0944</v>
+      </c>
+      <c r="E52" s="6">
+        <v>3374.99</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G52" s="6">
+        <v>9230.56</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53" s="10">
+        <v>1898.0944</v>
+      </c>
+      <c r="E53" s="10">
+        <v>3374.99</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G53" s="10">
+        <v>9421.06</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D54" s="6">
+        <v>1898.0944</v>
+      </c>
+      <c r="E54" s="6">
+        <v>3374.99</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G54" s="6">
+        <v>9584.36</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="10">
+        <v>1898.0944</v>
+      </c>
+      <c r="E55" s="10">
+        <v>3374.99</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G55" s="10">
+        <v>9715.9</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I55" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" s="6">
+        <v>486.70659999999998</v>
+      </c>
+      <c r="E56" s="6">
+        <v>782.99</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G56" s="6">
+        <v>8976.5499999999993</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D57" s="10">
+        <v>486.70659999999998</v>
+      </c>
+      <c r="E57" s="10">
+        <v>782.99</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="10">
+        <v>9026.44</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D58" s="6">
+        <v>486.70659999999998</v>
+      </c>
+      <c r="E58" s="6">
+        <v>782.99</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G58" s="6">
+        <v>9071.7999999999993</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D59" s="10">
+        <v>486.70659999999998</v>
+      </c>
+      <c r="E59" s="10">
+        <v>782.99</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G59" s="10">
+        <v>8513.8799999999992</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D60" s="6">
+        <v>486.70659999999998</v>
+      </c>
+      <c r="E60" s="6">
+        <v>782.99</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G60" s="6">
+        <v>8677.18</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D61" s="10">
+        <v>486.70659999999998</v>
+      </c>
+      <c r="E61" s="10">
+        <v>782.99</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G61" s="10">
+        <v>8808.7199999999993</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" s="6">
+        <v>486.70659999999998</v>
+      </c>
+      <c r="E62" s="6">
+        <v>782.99</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G62" s="6">
+        <v>8976.5499999999993</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I62" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" s="10">
+        <v>486.70659999999998</v>
+      </c>
+      <c r="E63" s="10">
+        <v>782.99</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" s="10">
+        <v>9026.44</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I63" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" s="6">
+        <v>486.70659999999998</v>
+      </c>
+      <c r="E64" s="6">
+        <v>782.99</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G64" s="6">
+        <v>9071.7999999999993</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D65" s="10">
+        <v>486.70659999999998</v>
+      </c>
+      <c r="E65" s="10">
+        <v>782.99</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G65" s="10">
+        <v>8513.8799999999992</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D66" s="6">
+        <v>486.70659999999998</v>
+      </c>
+      <c r="E66" s="6">
+        <v>782.99</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G66" s="6">
+        <v>8677.18</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D67" s="10">
+        <v>486.70659999999998</v>
+      </c>
+      <c r="E67" s="10">
+        <v>782.99</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G67" s="10">
+        <v>8808.7199999999993</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I67" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D68" s="6">
+        <v>187.15710000000001</v>
+      </c>
+      <c r="E68" s="6">
+        <v>337.22</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G68" s="6">
+        <v>1052.33</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="8" t="s">
+        <v>568</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D69" s="10">
+        <v>187.15710000000001</v>
+      </c>
+      <c r="E69" s="10">
+        <v>337.22</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G69" s="10">
+        <v>1070.47</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D70" s="6">
+        <v>187.15710000000001</v>
+      </c>
+      <c r="E70" s="6">
+        <v>337.22</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G70" s="6">
+        <v>1088.6199999999999</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I70" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D71" s="10">
+        <v>187.15710000000001</v>
+      </c>
+      <c r="E71" s="10">
+        <v>337.22</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G71" s="10">
+        <v>1115.83</v>
+      </c>
+      <c r="H71" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I71" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D72" s="6">
+        <v>187.15710000000001</v>
+      </c>
+      <c r="E72" s="6">
+        <v>337.22</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" s="6">
+        <v>1124.9000000000001</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="12" t="s">
+        <v>576</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>577</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D73" s="14">
+        <v>187.15710000000001</v>
+      </c>
+      <c r="E73" s="14">
+        <v>337.22</v>
+      </c>
+      <c r="F73" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G73" s="14">
+        <v>1133.98</v>
+      </c>
+      <c r="H73" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="I73" s="15" t="s">
+        <v>446</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911E74FC-E6C2-48E7-95D7-4F59C95716C5}">
   <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4613,7 +6727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>117</v>
       </c>
@@ -4642,7 +6756,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>119</v>
       </c>
@@ -4671,7 +6785,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>121</v>
       </c>
@@ -4700,7 +6814,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>123</v>
       </c>
@@ -4729,7 +6843,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>125</v>
       </c>
@@ -4758,7 +6872,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>127</v>
       </c>
@@ -4787,7 +6901,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>129</v>
       </c>
@@ -4816,7 +6930,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>132</v>
       </c>
@@ -4845,7 +6959,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>134</v>
       </c>
@@ -4874,7 +6988,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>136</v>
       </c>
@@ -4903,7 +7017,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>138</v>
       </c>
@@ -4932,7 +7046,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>140</v>
       </c>
@@ -4961,7 +7075,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>142</v>
       </c>
@@ -4990,7 +7104,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>144</v>
       </c>
@@ -5019,7 +7133,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>146</v>
       </c>
@@ -5048,7 +7162,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>148</v>
       </c>
@@ -5077,7 +7191,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>432</v>
       </c>
@@ -5100,7 +7214,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>434</v>
       </c>
@@ -5123,7 +7237,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>436</v>
       </c>
@@ -5146,7 +7260,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>438</v>
       </c>
@@ -5169,7 +7283,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>440</v>
       </c>
@@ -5192,7 +7306,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>442</v>
       </c>
@@ -5215,7 +7329,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>444</v>
       </c>
@@ -5244,7 +7358,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>447</v>
       </c>
@@ -5273,7 +7387,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>449</v>
       </c>
@@ -5302,7 +7416,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>451</v>
       </c>
@@ -5331,7 +7445,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>453</v>
       </c>
@@ -5360,7 +7474,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>455</v>
       </c>
@@ -5389,7 +7503,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>457</v>
       </c>
@@ -5418,7 +7532,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>459</v>
       </c>
@@ -5447,7 +7561,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>461</v>
       </c>
@@ -5476,7 +7590,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>612</v>
       </c>
@@ -5503,7 +7617,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>615</v>
       </c>
@@ -5530,7 +7644,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>617</v>
       </c>
@@ -5557,7 +7671,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>619</v>
       </c>
@@ -5584,7 +7698,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>621</v>
       </c>
@@ -5611,7 +7725,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>623</v>
       </c>
@@ -5638,7 +7752,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>625</v>
       </c>
@@ -5665,7 +7779,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>272</v>
       </c>
@@ -5690,7 +7804,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>276</v>
       </c>
@@ -5713,7 +7827,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>279</v>
       </c>
@@ -5736,7 +7850,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>282</v>
       </c>
@@ -5759,7 +7873,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>284</v>
       </c>
@@ -5782,7 +7896,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>287</v>
       </c>
@@ -5805,7 +7919,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>289</v>
       </c>
@@ -5828,7 +7942,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>627</v>
       </c>
@@ -5855,7 +7969,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>629</v>
       </c>
@@ -5882,7 +7996,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
         <v>631</v>
       </c>
@@ -5909,7 +8023,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>633</v>
       </c>
@@ -5936,7 +8050,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
         <v>636</v>
       </c>
@@ -5963,7 +8077,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>638</v>
       </c>
@@ -5990,7 +8104,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
         <v>640</v>
       </c>
@@ -6017,7 +8131,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>644</v>
       </c>
@@ -6044,7 +8158,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>646</v>
       </c>
@@ -6071,7 +8185,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>463</v>
       </c>
@@ -6096,7 +8210,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>466</v>
       </c>
@@ -6121,7 +8235,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>468</v>
       </c>
@@ -6146,7 +8260,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>470</v>
       </c>
@@ -6173,7 +8287,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>472</v>
       </c>
@@ -6200,7 +8314,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
         <v>474</v>
       </c>
@@ -6227,7 +8341,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>476</v>
       </c>
@@ -6252,7 +8366,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
         <v>478</v>
       </c>
@@ -6281,7 +8395,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>480</v>
       </c>
@@ -6310,7 +8424,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
         <v>482</v>
       </c>
@@ -6339,7 +8453,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>484</v>
       </c>
@@ -6368,7 +8482,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
         <v>486</v>
       </c>
@@ -6393,7 +8507,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>488</v>
       </c>
@@ -6418,7 +8532,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>490</v>
       </c>
@@ -6443,7 +8557,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>492</v>
       </c>
@@ -6470,7 +8584,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
         <v>494</v>
       </c>
@@ -6497,7 +8611,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>496</v>
       </c>
@@ -6524,7 +8638,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
         <v>498</v>
       </c>
@@ -6549,7 +8663,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>500</v>
       </c>
@@ -6572,7 +8686,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
         <v>503</v>
       </c>
@@ -6595,7 +8709,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>505</v>
       </c>
@@ -6618,7 +8732,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
         <v>507</v>
       </c>
@@ -6641,7 +8755,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>510</v>
       </c>
@@ -6664,7 +8778,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
         <v>512</v>
       </c>
@@ -6687,7 +8801,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>150</v>
       </c>
@@ -6716,7 +8830,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
         <v>152</v>
       </c>
@@ -6745,7 +8859,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>154</v>
       </c>
@@ -6774,7 +8888,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
         <v>156</v>
       </c>
@@ -6803,7 +8917,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>158</v>
       </c>
@@ -6832,7 +8946,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
         <v>160</v>
       </c>
@@ -6861,7 +8975,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="16" t="s">
         <v>162</v>
       </c>
@@ -6891,22 +9005,23 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F380E4CE-8028-43D3-8112-05D68DFC337D}">
   <dimension ref="A1:I137"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6935,7 +9050,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>578</v>
       </c>
@@ -6962,7 +9077,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>583</v>
       </c>
@@ -6989,7 +9104,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>586</v>
       </c>
@@ -7016,7 +9131,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>589</v>
       </c>
@@ -7043,7 +9158,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>592</v>
       </c>
@@ -7070,7 +9185,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>594</v>
       </c>
@@ -7097,7 +9212,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>225</v>
       </c>
@@ -7120,7 +9235,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>229</v>
       </c>
@@ -7143,7 +9258,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>231</v>
       </c>
@@ -7166,7 +9281,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>233</v>
       </c>
@@ -7189,7 +9304,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>596</v>
       </c>
@@ -7216,7 +9331,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>600</v>
       </c>
@@ -7243,7 +9358,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>236</v>
       </c>
@@ -7266,7 +9381,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>239</v>
       </c>
@@ -7289,7 +9404,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>242</v>
       </c>
@@ -7312,7 +9427,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>245</v>
       </c>
@@ -7335,7 +9450,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>248</v>
       </c>
@@ -7362,7 +9477,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>602</v>
       </c>
@@ -7389,7 +9504,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>605</v>
       </c>
@@ -7416,7 +9531,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>607</v>
       </c>
@@ -7443,7 +9558,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>609</v>
       </c>
@@ -7470,7 +9585,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>298</v>
       </c>
@@ -7499,7 +9614,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>302</v>
       </c>
@@ -7528,7 +9643,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>304</v>
       </c>
@@ -7557,7 +9672,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>306</v>
       </c>
@@ -7586,7 +9701,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>308</v>
       </c>
@@ -7615,7 +9730,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>310</v>
       </c>
@@ -7644,7 +9759,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>312</v>
       </c>
@@ -7673,7 +9788,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>314</v>
       </c>
@@ -7702,7 +9817,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>316</v>
       </c>
@@ -7731,7 +9846,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>318</v>
       </c>
@@ -7758,7 +9873,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>321</v>
       </c>
@@ -7787,7 +9902,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>323</v>
       </c>
@@ -7816,7 +9931,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>325</v>
       </c>
@@ -7845,7 +9960,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>327</v>
       </c>
@@ -7874,7 +9989,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>329</v>
       </c>
@@ -7903,7 +10018,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>331</v>
       </c>
@@ -7932,7 +10047,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>333</v>
       </c>
@@ -7961,7 +10076,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>335</v>
       </c>
@@ -7990,7 +10105,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>337</v>
       </c>
@@ -8019,7 +10134,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>339</v>
       </c>
@@ -8048,7 +10163,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>342</v>
       </c>
@@ -8077,7 +10192,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>344</v>
       </c>
@@ -8106,7 +10221,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>346</v>
       </c>
@@ -8133,7 +10248,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>349</v>
       </c>
@@ -8156,7 +10271,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>352</v>
       </c>
@@ -8179,7 +10294,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>354</v>
       </c>
@@ -8202,7 +10317,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
         <v>356</v>
       </c>
@@ -8225,7 +10340,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>358</v>
       </c>
@@ -8248,7 +10363,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
         <v>360</v>
       </c>
@@ -8271,7 +10386,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>362</v>
       </c>
@@ -8294,7 +10409,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
         <v>364</v>
       </c>
@@ -8317,7 +10432,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>366</v>
       </c>
@@ -8340,7 +10455,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>368</v>
       </c>
@@ -8369,7 +10484,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>370</v>
       </c>
@@ -8398,7 +10513,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>372</v>
       </c>
@@ -8427,7 +10542,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>374</v>
       </c>
@@ -8456,7 +10571,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>252</v>
       </c>
@@ -8479,7 +10594,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>254</v>
       </c>
@@ -8502,7 +10617,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
         <v>256</v>
       </c>
@@ -8525,7 +10640,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>376</v>
       </c>
@@ -8554,7 +10669,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
         <v>378</v>
       </c>
@@ -8583,7 +10698,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>380</v>
       </c>
@@ -8612,7 +10727,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
         <v>382</v>
       </c>
@@ -8641,7 +10756,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>258</v>
       </c>
@@ -8664,7 +10779,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
         <v>260</v>
       </c>
@@ -8687,7 +10802,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>262</v>
       </c>
@@ -8710,7 +10825,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>264</v>
       </c>
@@ -8733,7 +10848,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>266</v>
       </c>
@@ -8756,7 +10871,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
         <v>268</v>
       </c>
@@ -8779,7 +10894,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>270</v>
       </c>
@@ -8802,7 +10917,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
         <v>384</v>
       </c>
@@ -8829,7 +10944,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>388</v>
       </c>
@@ -8856,7 +10971,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
         <v>390</v>
       </c>
@@ -8883,7 +10998,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>392</v>
       </c>
@@ -8910,7 +11025,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
         <v>394</v>
       </c>
@@ -8937,7 +11052,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>396</v>
       </c>
@@ -8964,7 +11079,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
         <v>398</v>
       </c>
@@ -8989,7 +11104,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>400</v>
       </c>
@@ -9018,7 +11133,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
         <v>402</v>
       </c>
@@ -9047,7 +11162,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>404</v>
       </c>
@@ -9076,7 +11191,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
         <v>406</v>
       </c>
@@ -9103,7 +11218,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>408</v>
       </c>
@@ -9126,7 +11241,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
         <v>411</v>
       </c>
@@ -9149,7 +11264,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>413</v>
       </c>
@@ -9176,7 +11291,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
         <v>415</v>
       </c>
@@ -9203,7 +11318,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>418</v>
       </c>
@@ -9230,7 +11345,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="s">
         <v>420</v>
       </c>
@@ -9257,7 +11372,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>422</v>
       </c>
@@ -9282,7 +11397,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
         <v>9</v>
       </c>
@@ -9311,7 +11426,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>15</v>
       </c>
@@ -9340,7 +11455,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="8" t="s">
         <v>19</v>
       </c>
@@ -9369,7 +11484,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>22</v>
       </c>
@@ -9398,7 +11513,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="8" t="s">
         <v>25</v>
       </c>
@@ -9427,7 +11542,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>27</v>
       </c>
@@ -9456,7 +11571,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="8" t="s">
         <v>29</v>
       </c>
@@ -9485,7 +11600,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>32</v>
       </c>
@@ -9514,7 +11629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="8" t="s">
         <v>35</v>
       </c>
@@ -9543,7 +11658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>38</v>
       </c>
@@ -9572,7 +11687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="8" t="s">
         <v>40</v>
       </c>
@@ -9601,7 +11716,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
         <v>42</v>
       </c>
@@ -9630,7 +11745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="8" t="s">
         <v>44</v>
       </c>
@@ -9659,7 +11774,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>46</v>
       </c>
@@ -9688,7 +11803,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="8" t="s">
         <v>48</v>
       </c>
@@ -9717,7 +11832,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
         <v>50</v>
       </c>
@@ -9746,7 +11861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="8" t="s">
         <v>52</v>
       </c>
@@ -9775,7 +11890,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
         <v>54</v>
       </c>
@@ -9804,7 +11919,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="8" t="s">
         <v>56</v>
       </c>
@@ -9833,7 +11948,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>58</v>
       </c>
@@ -9862,7 +11977,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="8" t="s">
         <v>60</v>
       </c>
@@ -9891,7 +12006,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>64</v>
       </c>
@@ -9920,7 +12035,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="8" t="s">
         <v>67</v>
       </c>
@@ -9949,7 +12064,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
         <v>69</v>
       </c>
@@ -9978,7 +12093,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="8" t="s">
         <v>72</v>
       </c>
@@ -10007,7 +12122,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
         <v>75</v>
       </c>
@@ -10036,7 +12151,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="8" t="s">
         <v>77</v>
       </c>
@@ -10065,7 +12180,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
         <v>79</v>
       </c>
@@ -10094,7 +12209,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="8" t="s">
         <v>84</v>
       </c>
@@ -10123,7 +12238,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
         <v>86</v>
       </c>
@@ -10152,7 +12267,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="8" t="s">
         <v>88</v>
       </c>
@@ -10181,7 +12296,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
         <v>90</v>
       </c>
@@ -10210,7 +12325,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="8" t="s">
         <v>92</v>
       </c>
@@ -10239,7 +12354,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
         <v>94</v>
       </c>
@@ -10268,7 +12383,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="8" t="s">
         <v>96</v>
       </c>
@@ -10297,7 +12412,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
         <v>98</v>
       </c>
@@ -10326,7 +12441,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="8" t="s">
         <v>101</v>
       </c>
@@ -10355,7 +12470,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="4" t="s">
         <v>103</v>
       </c>
@@ -10384,7 +12499,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
         <v>105</v>
       </c>
@@ -10413,7 +12528,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="4" t="s">
         <v>107</v>
       </c>
@@ -10442,7 +12557,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
         <v>109</v>
       </c>
@@ -10471,7 +12586,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
         <v>425</v>
       </c>
@@ -10496,7 +12611,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="8" t="s">
         <v>428</v>
       </c>
@@ -10521,7 +12636,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
         <v>430</v>
       </c>
@@ -10546,7 +12661,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="8" t="s">
         <v>111</v>
       </c>
@@ -10575,7 +12690,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
         <v>113</v>
       </c>
@@ -10604,7 +12719,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="12" t="s">
         <v>115</v>
       </c>
@@ -10634,6 +12749,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>